<commit_message>
cuadro precios temporada (año) finalizado
</commit_message>
<xml_diff>
--- a/ptdataknow/entrenamiento_local/proyecciones de cada materia para cada tiempo.xlsx
+++ b/ptdataknow/entrenamiento_local/proyecciones de cada materia para cada tiempo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quint.LAPTOP-LGVR2QRN\OneDrive - correounivalle.edu.co\Docs_OneDrive\ian-peña-cientificos\CIBERSEGURIDAD_SERES_ETICOS\graphs_gif\classical_trajectory\ptdataknow\entrenamiento_local\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54075440-DC60-4744-88C2-187110BB2CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05185FD-0289-4BC4-8777-2D21CF8D4810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>X</t>
   </si>
@@ -58,13 +58,37 @@
   </si>
   <si>
     <t>3 Años</t>
+  </si>
+  <si>
+    <t>89.18</t>
+  </si>
+  <si>
+    <t>82.79</t>
+  </si>
+  <si>
+    <t>88.20</t>
+  </si>
+  <si>
+    <t>79.52</t>
+  </si>
+  <si>
+    <t>2165.25</t>
+  </si>
+  <si>
+    <t>1834.14</t>
+  </si>
+  <si>
+    <t>2246.75</t>
+  </si>
+  <si>
+    <t>2483.45</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +105,12 @@
       <sz val="11"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -118,12 +148,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,66 +436,83 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update proyecciones de cada materia para cada tiempo.xlsx
</commit_message>
<xml_diff>
--- a/ptdataknow/entrenamiento_local/proyecciones de cada materia para cada tiempo.xlsx
+++ b/ptdataknow/entrenamiento_local/proyecciones de cada materia para cada tiempo.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quint.LAPTOP-LGVR2QRN\OneDrive - correounivalle.edu.co\Docs_OneDrive\ian-peña-cientificos\CIBERSEGURIDAD_SERES_ETICOS\graphs_gif\classical_trajectory\ptdataknow\entrenamiento_local\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A336F2-6E10-4BD3-94C9-9A831BEEE17E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E0DBA68-5BEB-4F7E-80BA-4D56F93104F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>X</t>
   </si>
@@ -36,18 +47,6 @@
     <t>Z</t>
   </si>
   <si>
-    <t>547.33</t>
-  </si>
-  <si>
-    <t>614.07</t>
-  </si>
-  <si>
-    <t>589.30</t>
-  </si>
-  <si>
-    <t>568.93</t>
-  </si>
-  <si>
     <t>0 Años</t>
   </si>
   <si>
@@ -60,40 +59,22 @@
     <t>3 Años</t>
   </si>
   <si>
-    <t>89.18</t>
-  </si>
-  <si>
-    <t>82.79</t>
-  </si>
-  <si>
-    <t>88.20</t>
-  </si>
-  <si>
-    <t>79.52</t>
-  </si>
-  <si>
-    <t>2165.25</t>
-  </si>
-  <si>
-    <t>1834.14</t>
-  </si>
-  <si>
-    <t>2246.75</t>
-  </si>
-  <si>
-    <t>2483.45</t>
-  </si>
-  <si>
     <t>Equipo 1</t>
   </si>
   <si>
     <t>Equipo 2</t>
+  </si>
+  <si>
+    <t>total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.000"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -119,15 +100,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -150,15 +137,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,79 +458,153 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>89.18</v>
+      </c>
+      <c r="C2" s="3">
+        <v>82.79</v>
+      </c>
+      <c r="D2" s="3">
+        <v>88.2</v>
+      </c>
+      <c r="E2" s="3">
+        <v>79.52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>547.33000000000004</v>
+      </c>
+      <c r="C3" s="3">
+        <v>614.07000000000005</v>
+      </c>
+      <c r="D3" s="3">
+        <v>589.29999999999995</v>
+      </c>
+      <c r="E3" s="3">
+        <v>568.92999999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2165.25</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1834.14</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2246.75</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2483.4499999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="B8" s="5">
+        <f xml:space="preserve"> (0.2)*B2 + 0.8*B3</f>
+        <v>455.70000000000005</v>
+      </c>
+      <c r="C8" s="5">
+        <f t="shared" ref="C8:E8" si="0" xml:space="preserve"> (0.2)*C2 + 0.8*C3</f>
+        <v>507.81400000000008</v>
+      </c>
+      <c r="D8" s="5">
+        <f t="shared" si="0"/>
+        <v>489.08</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="0"/>
+        <v>471.048</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="B9" s="5">
+        <f xml:space="preserve"> (1/3)*B2+(1/3)*B3+(1/3)*B4</f>
+        <v>933.92</v>
+      </c>
+      <c r="C9" s="5">
+        <f t="shared" ref="C9:E9" si="1" xml:space="preserve"> (1/3)*C2+(1/3)*C3+(1/3)*C4</f>
+        <v>843.66666666666663</v>
+      </c>
+      <c r="D9" s="5">
+        <f t="shared" si="1"/>
+        <v>974.75</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" si="1"/>
+        <v>1043.9666666666667</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>20</v>
+      <c r="B11" s="5">
+        <f>B8+B9</f>
+        <v>1389.62</v>
+      </c>
+      <c r="C11" s="5">
+        <f t="shared" ref="C11:E11" si="2">C8+C9</f>
+        <v>1351.4806666666668</v>
+      </c>
+      <c r="D11" s="5">
+        <f t="shared" si="2"/>
+        <v>1463.83</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" si="2"/>
+        <v>1515.0146666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>